<commit_message>
Grans canvis en lectura prototipus()
</commit_message>
<xml_diff>
--- a/conductor_DataHarmonization.xlsx
+++ b/conductor_DataHarmonization.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="192">
   <si>
     <t>id</t>
   </si>
@@ -428,21 +428,6 @@
     <t>Not matching</t>
   </si>
   <si>
-    <t>exc_cancer</t>
-  </si>
-  <si>
-    <t>exc_prev_CVD</t>
-  </si>
-  <si>
-    <t>exc_prev_KD</t>
-  </si>
-  <si>
-    <t>exc_prev_MET</t>
-  </si>
-  <si>
-    <t>exc_post</t>
-  </si>
-  <si>
     <t>exc_apestat</t>
   </si>
   <si>
@@ -512,9 +497,6 @@
     <t xml:space="preserve">Prescripciones.Tiazolinadionas / [A10BG**]. </t>
   </si>
   <si>
-    <t>exclusio1_prev</t>
-  </si>
-  <si>
     <t>Exclusion antes 31.12.2018</t>
   </si>
   <si>
@@ -572,16 +554,43 @@
     <t>7</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
     <t>exc_post2</t>
   </si>
   <si>
-    <t>13</t>
+    <t>exclusio1_prev_2018</t>
+  </si>
+  <si>
+    <t>DG.cancer</t>
+  </si>
+  <si>
+    <t>DG.prevalent_CVD</t>
+  </si>
+  <si>
+    <t>DG.prevalent_KD</t>
+  </si>
+  <si>
+    <t>DG.prevalent_MET</t>
+  </si>
+  <si>
+    <t>exc_antiguitat</t>
+  </si>
+  <si>
+    <t>exc_post1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
   </si>
 </sst>
 </file>
@@ -677,7 +686,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -756,6 +765,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="22">
     <border>
@@ -1020,7 +1035,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1341,22 +1356,31 @@
     <xf numFmtId="49" fontId="11" fillId="12" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="13" borderId="21" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="11" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="14" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="12" fillId="14" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="12" fillId="14" borderId="21" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1637,19 +1661,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L74"/>
+  <dimension ref="A1:L75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="82" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" style="82" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" style="82" customWidth="1"/>
     <col min="3" max="3" width="107" style="82" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" style="87" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" style="87" customWidth="1"/>
@@ -1658,8 +1682,7 @@
     <col min="8" max="8" width="19.85546875" style="88" customWidth="1"/>
     <col min="9" max="9" width="18.85546875" style="124" customWidth="1"/>
     <col min="10" max="10" width="16.85546875" style="124" customWidth="1"/>
-    <col min="11" max="11" width="16.42578125" style="124" customWidth="1"/>
-    <col min="12" max="12" width="20.28515625" style="92" customWidth="1"/>
+    <col min="11" max="12" width="16.42578125" style="124" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="90"/>
   </cols>
   <sheetData>
@@ -1683,7 +1706,7 @@
         <v>104</v>
       </c>
       <c r="G1" s="118" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="H1" s="86" t="s">
         <v>132</v>
@@ -1695,10 +1718,10 @@
         <v>134</v>
       </c>
       <c r="K1" s="123" t="s">
-        <v>141</v>
+        <v>186</v>
       </c>
       <c r="L1" s="123" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="16.5">
@@ -1799,10 +1822,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="82" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="C8" s="82" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G8" s="118">
         <v>1</v>
@@ -1811,66 +1834,66 @@
     <row r="9" spans="1:12" s="117" customFormat="1" ht="16.5">
       <c r="A9" s="113"/>
       <c r="B9" s="114" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C9" s="114" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="D9" s="115"/>
       <c r="E9" s="115"/>
       <c r="F9" s="115"/>
-      <c r="G9" s="119"/>
+      <c r="G9" s="119">
+        <v>1</v>
+      </c>
       <c r="H9" s="116"/>
       <c r="I9" s="125"/>
       <c r="J9" s="125"/>
       <c r="K9" s="125"/>
-      <c r="L9" s="120"/>
+      <c r="L9" s="125"/>
     </row>
     <row r="10" spans="1:12" ht="16.5">
       <c r="A10" s="83"/>
       <c r="B10" s="82" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="C10" s="82" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="16.5">
       <c r="A11" s="83"/>
       <c r="B11" s="82" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C11" s="82" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:12" s="117" customFormat="1" ht="16.5">
       <c r="A12" s="113"/>
       <c r="B12" s="114" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C12" s="114" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D12" s="115"/>
       <c r="E12" s="115"/>
       <c r="F12" s="115"/>
-      <c r="G12" s="120">
-        <v>1</v>
-      </c>
+      <c r="G12" s="120"/>
       <c r="H12" s="116"/>
       <c r="I12" s="125"/>
       <c r="J12" s="125"/>
       <c r="K12" s="125"/>
-      <c r="L12" s="120"/>
+      <c r="L12" s="125"/>
     </row>
     <row r="13" spans="1:12" ht="16.5">
       <c r="A13" s="83"/>
       <c r="B13" s="82" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C13" s="82" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:12" s="97" customFormat="1" ht="16.5">
@@ -1893,7 +1916,7 @@
       <c r="I14" s="126"/>
       <c r="J14" s="126"/>
       <c r="K14" s="126"/>
-      <c r="L14" s="121"/>
+      <c r="L14" s="126"/>
     </row>
     <row r="15" spans="1:12" s="97" customFormat="1" ht="16.5">
       <c r="A15" s="93">
@@ -1915,7 +1938,7 @@
       <c r="I15" s="126"/>
       <c r="J15" s="126"/>
       <c r="K15" s="126"/>
-      <c r="L15" s="121"/>
+      <c r="L15" s="126"/>
     </row>
     <row r="16" spans="1:12" s="97" customFormat="1" ht="16.5">
       <c r="A16" s="93">
@@ -1937,7 +1960,7 @@
       <c r="I16" s="126"/>
       <c r="J16" s="126"/>
       <c r="K16" s="126"/>
-      <c r="L16" s="121"/>
+      <c r="L16" s="126"/>
     </row>
     <row r="17" spans="1:12" s="97" customFormat="1" ht="16.5">
       <c r="A17" s="93">
@@ -1959,7 +1982,7 @@
       <c r="I17" s="126"/>
       <c r="J17" s="126"/>
       <c r="K17" s="126"/>
-      <c r="L17" s="121"/>
+      <c r="L17" s="126"/>
     </row>
     <row r="18" spans="1:12" s="97" customFormat="1" ht="16.5">
       <c r="A18" s="93">
@@ -1981,7 +2004,7 @@
       <c r="I18" s="126"/>
       <c r="J18" s="126"/>
       <c r="K18" s="126"/>
-      <c r="L18" s="121"/>
+      <c r="L18" s="126"/>
     </row>
     <row r="19" spans="1:12" s="97" customFormat="1" ht="16.5">
       <c r="A19" s="93">
@@ -2005,7 +2028,7 @@
       <c r="I19" s="126"/>
       <c r="J19" s="126"/>
       <c r="K19" s="126"/>
-      <c r="L19" s="121"/>
+      <c r="L19" s="126"/>
     </row>
     <row r="20" spans="1:12" s="97" customFormat="1" ht="16.5">
       <c r="A20" s="93">
@@ -2025,7 +2048,7 @@
       <c r="I20" s="126"/>
       <c r="J20" s="126"/>
       <c r="K20" s="126"/>
-      <c r="L20" s="121"/>
+      <c r="L20" s="126"/>
     </row>
     <row r="21" spans="1:12" s="97" customFormat="1" ht="16.5">
       <c r="A21" s="93">
@@ -2047,7 +2070,7 @@
       <c r="I21" s="126"/>
       <c r="J21" s="126"/>
       <c r="K21" s="126"/>
-      <c r="L21" s="121"/>
+      <c r="L21" s="126"/>
     </row>
     <row r="22" spans="1:12" s="97" customFormat="1" ht="16.5">
       <c r="A22" s="93">
@@ -2069,7 +2092,7 @@
       <c r="I22" s="126"/>
       <c r="J22" s="126"/>
       <c r="K22" s="126"/>
-      <c r="L22" s="121"/>
+      <c r="L22" s="126"/>
     </row>
     <row r="23" spans="1:12" ht="16.5">
       <c r="A23" s="83">
@@ -2168,14 +2191,14 @@
       <c r="I30" s="127"/>
       <c r="J30" s="127"/>
       <c r="K30" s="127"/>
-      <c r="L30" s="122"/>
+      <c r="L30" s="127"/>
     </row>
     <row r="31" spans="1:12" s="105" customFormat="1" ht="16.5">
       <c r="A31" s="100">
         <v>24</v>
       </c>
       <c r="B31" s="101" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C31" s="102" t="s">
         <v>78</v>
@@ -2190,7 +2213,7 @@
       <c r="I31" s="127"/>
       <c r="J31" s="127"/>
       <c r="K31" s="127"/>
-      <c r="L31" s="122"/>
+      <c r="L31" s="127"/>
     </row>
     <row r="32" spans="1:12" s="105" customFormat="1" ht="16.5">
       <c r="A32" s="100">
@@ -2212,7 +2235,7 @@
       <c r="I32" s="127"/>
       <c r="J32" s="127"/>
       <c r="K32" s="127"/>
-      <c r="L32" s="122"/>
+      <c r="L32" s="127"/>
     </row>
     <row r="33" spans="1:12" s="105" customFormat="1" ht="16.5">
       <c r="A33" s="100">
@@ -2234,14 +2257,14 @@
       <c r="I33" s="127"/>
       <c r="J33" s="127"/>
       <c r="K33" s="127"/>
-      <c r="L33" s="122"/>
+      <c r="L33" s="127"/>
     </row>
     <row r="34" spans="1:12" s="105" customFormat="1" ht="16.5">
       <c r="A34" s="100">
         <v>27</v>
       </c>
       <c r="B34" s="101" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C34" s="102" t="s">
         <v>81</v>
@@ -2256,7 +2279,7 @@
       <c r="I34" s="127"/>
       <c r="J34" s="127"/>
       <c r="K34" s="127"/>
-      <c r="L34" s="122"/>
+      <c r="L34" s="127"/>
     </row>
     <row r="35" spans="1:12" s="105" customFormat="1" ht="16.5">
       <c r="A35" s="100">
@@ -2278,14 +2301,14 @@
       <c r="I35" s="127"/>
       <c r="J35" s="127"/>
       <c r="K35" s="127"/>
-      <c r="L35" s="122"/>
+      <c r="L35" s="127"/>
     </row>
     <row r="36" spans="1:12" s="105" customFormat="1" ht="16.5">
       <c r="A36" s="100">
         <v>29</v>
       </c>
       <c r="B36" s="101" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C36" s="101" t="s">
         <v>83</v>
@@ -2300,14 +2323,14 @@
       <c r="I36" s="127"/>
       <c r="J36" s="127"/>
       <c r="K36" s="127"/>
-      <c r="L36" s="122"/>
+      <c r="L36" s="127"/>
     </row>
     <row r="37" spans="1:12" s="105" customFormat="1" ht="16.5">
       <c r="A37" s="100">
         <v>30</v>
       </c>
       <c r="B37" s="101" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C37" s="101" t="s">
         <v>84</v>
@@ -2322,17 +2345,17 @@
       <c r="I37" s="127"/>
       <c r="J37" s="127"/>
       <c r="K37" s="127"/>
-      <c r="L37" s="122"/>
+      <c r="L37" s="127"/>
     </row>
     <row r="38" spans="1:12" s="105" customFormat="1" ht="16.5">
       <c r="A38" s="100">
         <v>31</v>
       </c>
       <c r="B38" s="101" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C38" s="102" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D38" s="103"/>
       <c r="E38" s="103">
@@ -2344,14 +2367,14 @@
       <c r="I38" s="127"/>
       <c r="J38" s="127"/>
       <c r="K38" s="127"/>
-      <c r="L38" s="122"/>
+      <c r="L38" s="127"/>
     </row>
     <row r="39" spans="1:12" s="105" customFormat="1" ht="16.5">
       <c r="A39" s="100">
         <v>32</v>
       </c>
       <c r="B39" s="101" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C39" s="102" t="s">
         <v>85</v>
@@ -2366,17 +2389,17 @@
       <c r="I39" s="127"/>
       <c r="J39" s="127"/>
       <c r="K39" s="127"/>
-      <c r="L39" s="122"/>
+      <c r="L39" s="127"/>
     </row>
     <row r="40" spans="1:12" s="105" customFormat="1" ht="16.5">
       <c r="A40" s="100">
         <v>33</v>
       </c>
       <c r="B40" s="101" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C40" s="101" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D40" s="103"/>
       <c r="E40" s="103">
@@ -2388,7 +2411,7 @@
       <c r="I40" s="127"/>
       <c r="J40" s="127"/>
       <c r="K40" s="127"/>
-      <c r="L40" s="122"/>
+      <c r="L40" s="127"/>
     </row>
     <row r="41" spans="1:12" s="105" customFormat="1" ht="16.5">
       <c r="A41" s="100">
@@ -2410,7 +2433,7 @@
       <c r="I41" s="127"/>
       <c r="J41" s="127"/>
       <c r="K41" s="127"/>
-      <c r="L41" s="122"/>
+      <c r="L41" s="127"/>
     </row>
     <row r="42" spans="1:12" s="105" customFormat="1" ht="16.5">
       <c r="A42" s="100">
@@ -2432,7 +2455,7 @@
       <c r="I42" s="127"/>
       <c r="J42" s="127"/>
       <c r="K42" s="127"/>
-      <c r="L42" s="122"/>
+      <c r="L42" s="127"/>
     </row>
     <row r="43" spans="1:12" s="105" customFormat="1" ht="16.5">
       <c r="A43" s="100">
@@ -2454,7 +2477,7 @@
       <c r="I43" s="127"/>
       <c r="J43" s="127"/>
       <c r="K43" s="127"/>
-      <c r="L43" s="122"/>
+      <c r="L43" s="127"/>
     </row>
     <row r="44" spans="1:12" s="105" customFormat="1" ht="16.5">
       <c r="A44" s="100">
@@ -2476,7 +2499,7 @@
       <c r="I44" s="127"/>
       <c r="J44" s="127"/>
       <c r="K44" s="127"/>
-      <c r="L44" s="122"/>
+      <c r="L44" s="127"/>
     </row>
     <row r="45" spans="1:12" s="105" customFormat="1" ht="16.5">
       <c r="A45" s="100">
@@ -2498,7 +2521,7 @@
       <c r="I45" s="127"/>
       <c r="J45" s="127"/>
       <c r="K45" s="127"/>
-      <c r="L45" s="122"/>
+      <c r="L45" s="127"/>
     </row>
     <row r="46" spans="1:12" s="105" customFormat="1" ht="16.5">
       <c r="A46" s="100">
@@ -2520,7 +2543,7 @@
       <c r="I46" s="127"/>
       <c r="J46" s="127"/>
       <c r="K46" s="127"/>
-      <c r="L46" s="122"/>
+      <c r="L46" s="127"/>
     </row>
     <row r="47" spans="1:12" s="105" customFormat="1" ht="16.5">
       <c r="A47" s="100">
@@ -2542,7 +2565,7 @@
       <c r="I47" s="127"/>
       <c r="J47" s="127"/>
       <c r="K47" s="127"/>
-      <c r="L47" s="122"/>
+      <c r="L47" s="127"/>
     </row>
     <row r="48" spans="1:12" s="105" customFormat="1" ht="16.5">
       <c r="A48" s="100">
@@ -2564,7 +2587,7 @@
       <c r="I48" s="127"/>
       <c r="J48" s="127"/>
       <c r="K48" s="127"/>
-      <c r="L48" s="122"/>
+      <c r="L48" s="127"/>
     </row>
     <row r="49" spans="1:12" s="105" customFormat="1" ht="16.5">
       <c r="A49" s="100">
@@ -2586,7 +2609,7 @@
       <c r="I49" s="127"/>
       <c r="J49" s="127"/>
       <c r="K49" s="127"/>
-      <c r="L49" s="122"/>
+      <c r="L49" s="127"/>
     </row>
     <row r="50" spans="1:12" s="105" customFormat="1" ht="16.5">
       <c r="A50" s="100">
@@ -2608,7 +2631,7 @@
       <c r="I50" s="127"/>
       <c r="J50" s="127"/>
       <c r="K50" s="127"/>
-      <c r="L50" s="122"/>
+      <c r="L50" s="127"/>
     </row>
     <row r="51" spans="1:12" s="105" customFormat="1" ht="16.5">
       <c r="A51" s="100">
@@ -2630,7 +2653,7 @@
       <c r="I51" s="127"/>
       <c r="J51" s="127"/>
       <c r="K51" s="127"/>
-      <c r="L51" s="122"/>
+      <c r="L51" s="127"/>
     </row>
     <row r="52" spans="1:12" ht="16.5">
       <c r="A52" s="83">
@@ -2763,7 +2786,7 @@
         <v>110</v>
       </c>
       <c r="C61" s="82" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E61" s="87">
         <v>43</v>
@@ -2783,283 +2806,302 @@
         <v>44</v>
       </c>
     </row>
-    <row r="63" spans="1:12" s="110" customFormat="1" ht="16.5">
-      <c r="A63" s="106">
+    <row r="63" spans="1:12" s="134" customFormat="1" ht="16.5">
+      <c r="A63" s="128">
         <v>56</v>
       </c>
-      <c r="B63" s="107" t="s">
-        <v>165</v>
-      </c>
-      <c r="C63" s="107" t="s">
-        <v>166</v>
-      </c>
-      <c r="D63" s="108"/>
-      <c r="E63" s="108"/>
-      <c r="F63" s="108"/>
-      <c r="G63" s="111"/>
-      <c r="H63" s="109">
-        <v>1</v>
-      </c>
-      <c r="I63" s="128"/>
-      <c r="J63" s="128"/>
-      <c r="K63" s="112"/>
-      <c r="L63" s="111"/>
-    </row>
-    <row r="64" spans="1:12" s="110" customFormat="1" ht="16.5">
-      <c r="A64" s="106">
+      <c r="B63" s="129" t="s">
+        <v>180</v>
+      </c>
+      <c r="C63" s="129" t="s">
+        <v>160</v>
+      </c>
+      <c r="D63" s="130"/>
+      <c r="E63" s="130"/>
+      <c r="F63" s="130"/>
+      <c r="G63" s="131"/>
+      <c r="H63" s="132">
+        <v>1</v>
+      </c>
+      <c r="I63" s="133" t="s">
+        <v>177</v>
+      </c>
+      <c r="J63" s="133" t="s">
+        <v>177</v>
+      </c>
+      <c r="K63" s="133"/>
+      <c r="L63" s="133"/>
+    </row>
+    <row r="64" spans="1:12" s="134" customFormat="1" ht="16.5">
+      <c r="A64" s="128">
         <v>57</v>
       </c>
-      <c r="B64" s="107" t="s">
+      <c r="B64" s="129" t="s">
         <v>131</v>
       </c>
-      <c r="C64" s="107" t="s">
-        <v>152</v>
-      </c>
-      <c r="D64" s="108"/>
-      <c r="E64" s="108"/>
-      <c r="F64" s="108"/>
-      <c r="G64" s="111"/>
-      <c r="H64" s="109">
+      <c r="C64" s="129" t="s">
+        <v>147</v>
+      </c>
+      <c r="D64" s="130"/>
+      <c r="E64" s="130"/>
+      <c r="F64" s="130"/>
+      <c r="G64" s="131"/>
+      <c r="H64" s="132">
         <v>2</v>
       </c>
-      <c r="I64" s="112">
-        <v>1</v>
-      </c>
-      <c r="J64" s="112">
-        <v>1</v>
-      </c>
-      <c r="K64" s="112"/>
-      <c r="L64" s="111"/>
-    </row>
-    <row r="65" spans="1:12" s="110" customFormat="1" ht="16.5">
-      <c r="A65" s="106">
+      <c r="I64" s="133">
+        <v>1</v>
+      </c>
+      <c r="J64" s="133">
+        <v>1</v>
+      </c>
+      <c r="K64" s="133"/>
+      <c r="L64" s="133"/>
+    </row>
+    <row r="65" spans="1:12" s="134" customFormat="1" ht="16.5">
+      <c r="A65" s="128">
         <v>58</v>
       </c>
-      <c r="B65" s="107" t="s">
+      <c r="B65" s="129" t="s">
         <v>135</v>
       </c>
-      <c r="C65" s="107" t="s">
+      <c r="C65" s="129" t="s">
         <v>136</v>
       </c>
-      <c r="D65" s="108"/>
-      <c r="E65" s="108"/>
-      <c r="F65" s="108"/>
-      <c r="G65" s="111"/>
-      <c r="H65" s="109">
-        <v>8</v>
-      </c>
-      <c r="I65" s="128"/>
-      <c r="J65" s="112">
-        <v>1</v>
-      </c>
-      <c r="K65" s="112"/>
-      <c r="L65" s="111"/>
-    </row>
-    <row r="66" spans="1:12" s="133" customFormat="1" ht="16.5">
-      <c r="A66" s="130">
-        <v>59</v>
-      </c>
-      <c r="B66" s="131" t="s">
+      <c r="D65" s="130"/>
+      <c r="E65" s="130"/>
+      <c r="F65" s="130"/>
+      <c r="G65" s="131"/>
+      <c r="H65" s="132" t="s">
+        <v>188</v>
+      </c>
+      <c r="I65" s="135"/>
+      <c r="J65" s="133">
+        <v>1</v>
+      </c>
+      <c r="K65" s="133"/>
+      <c r="L65" s="133"/>
+    </row>
+    <row r="66" spans="1:12" s="110" customFormat="1" ht="16.5">
+      <c r="A66" s="106">
+        <v>63</v>
+      </c>
+      <c r="B66" s="107" t="s">
+        <v>138</v>
+      </c>
+      <c r="C66" s="107" t="s">
+        <v>146</v>
+      </c>
+      <c r="D66" s="108"/>
+      <c r="E66" s="108"/>
+      <c r="F66" s="108"/>
+      <c r="G66" s="111"/>
+      <c r="H66" s="109" t="s">
+        <v>177</v>
+      </c>
+      <c r="I66" s="112"/>
+      <c r="J66" s="112"/>
+      <c r="K66" s="112" t="s">
+        <v>177</v>
+      </c>
+      <c r="L66" s="112"/>
+    </row>
+    <row r="67" spans="1:12" s="110" customFormat="1" ht="16.5">
+      <c r="A67" s="106">
+        <v>66</v>
+      </c>
+      <c r="B67" s="107" t="s">
         <v>137</v>
       </c>
-      <c r="C66" s="131" t="s">
-        <v>146</v>
-      </c>
-      <c r="D66" s="120"/>
-      <c r="E66" s="120"/>
-      <c r="F66" s="120"/>
-      <c r="G66" s="120"/>
-      <c r="H66" s="132">
-        <v>4</v>
-      </c>
-      <c r="I66" s="132"/>
-      <c r="J66" s="132"/>
-      <c r="K66" s="132"/>
-      <c r="L66" s="120"/>
-    </row>
-    <row r="67" spans="1:12" s="133" customFormat="1" ht="16.5">
-      <c r="A67" s="130">
-        <v>60</v>
-      </c>
-      <c r="B67" s="131" t="s">
-        <v>138</v>
-      </c>
-      <c r="C67" s="131" t="s">
-        <v>147</v>
-      </c>
-      <c r="D67" s="120"/>
-      <c r="E67" s="120"/>
-      <c r="F67" s="120"/>
-      <c r="G67" s="120"/>
-      <c r="H67" s="132">
-        <v>5</v>
-      </c>
-      <c r="I67" s="132"/>
-      <c r="J67" s="132"/>
-      <c r="K67" s="132"/>
-      <c r="L67" s="120"/>
-    </row>
-    <row r="68" spans="1:12" s="133" customFormat="1" ht="16.5">
-      <c r="A68" s="130">
-        <v>61</v>
-      </c>
-      <c r="B68" s="131" t="s">
-        <v>139</v>
-      </c>
-      <c r="C68" s="131" t="s">
+      <c r="C67" s="107" t="s">
+        <v>145</v>
+      </c>
+      <c r="D67" s="108"/>
+      <c r="E67" s="108"/>
+      <c r="F67" s="108"/>
+      <c r="G67" s="111"/>
+      <c r="H67" s="109" t="s">
+        <v>191</v>
+      </c>
+      <c r="I67" s="112"/>
+      <c r="J67" s="112"/>
+      <c r="K67" s="112" t="s">
+        <v>177</v>
+      </c>
+      <c r="L67" s="112"/>
+    </row>
+    <row r="68" spans="1:12" s="110" customFormat="1" ht="16.5">
+      <c r="A68" s="106">
+        <v>67</v>
+      </c>
+      <c r="B68" s="107" t="s">
         <v>148</v>
       </c>
-      <c r="D68" s="120"/>
-      <c r="E68" s="120"/>
-      <c r="F68" s="120"/>
-      <c r="G68" s="120"/>
-      <c r="H68" s="132">
-        <v>6</v>
-      </c>
-      <c r="I68" s="132"/>
-      <c r="J68" s="132"/>
-      <c r="K68" s="132"/>
-      <c r="L68" s="120"/>
-    </row>
-    <row r="69" spans="1:12" s="133" customFormat="1" ht="16.5">
-      <c r="A69" s="130">
-        <v>62</v>
-      </c>
-      <c r="B69" s="131" t="s">
-        <v>140</v>
-      </c>
-      <c r="C69" s="131" t="s">
+      <c r="C68" s="107" t="s">
         <v>149</v>
       </c>
-      <c r="D69" s="120"/>
-      <c r="E69" s="120"/>
-      <c r="F69" s="120"/>
-      <c r="G69" s="120"/>
-      <c r="H69" s="132" t="s">
-        <v>184</v>
-      </c>
-      <c r="I69" s="132"/>
-      <c r="J69" s="132"/>
-      <c r="K69" s="132"/>
-      <c r="L69" s="120"/>
+      <c r="D68" s="108"/>
+      <c r="E68" s="108"/>
+      <c r="F68" s="108"/>
+      <c r="G68" s="111"/>
+      <c r="H68" s="109" t="s">
+        <v>178</v>
+      </c>
+      <c r="I68" s="112"/>
+      <c r="J68" s="112"/>
+      <c r="K68" s="112" t="s">
+        <v>177</v>
+      </c>
+      <c r="L68" s="112"/>
+    </row>
+    <row r="69" spans="1:12" s="110" customFormat="1" ht="16.5">
+      <c r="A69" s="106">
+        <v>69</v>
+      </c>
+      <c r="B69" s="107" t="s">
+        <v>181</v>
+      </c>
+      <c r="C69" s="107" t="s">
+        <v>141</v>
+      </c>
+      <c r="D69" s="108"/>
+      <c r="E69" s="108"/>
+      <c r="F69" s="108"/>
+      <c r="G69" s="111"/>
+      <c r="H69" s="109" t="s">
+        <v>187</v>
+      </c>
+      <c r="I69" s="112"/>
+      <c r="J69" s="112"/>
+      <c r="K69" s="112" t="s">
+        <v>177</v>
+      </c>
+      <c r="L69" s="112"/>
     </row>
     <row r="70" spans="1:12" s="110" customFormat="1" ht="16.5">
       <c r="A70" s="106">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="B70" s="107" t="s">
-        <v>143</v>
+        <v>182</v>
       </c>
       <c r="C70" s="107" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D70" s="108"/>
       <c r="E70" s="108"/>
       <c r="F70" s="108"/>
       <c r="G70" s="111"/>
-      <c r="H70" s="109">
-        <v>9</v>
+      <c r="H70" s="109" t="s">
+        <v>188</v>
       </c>
       <c r="I70" s="112"/>
       <c r="J70" s="112"/>
       <c r="K70" s="112" t="s">
-        <v>183</v>
-      </c>
-      <c r="L70" s="111"/>
+        <v>177</v>
+      </c>
+      <c r="L70" s="112"/>
     </row>
     <row r="71" spans="1:12" s="110" customFormat="1" ht="16.5">
       <c r="A71" s="106">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B71" s="107" t="s">
-        <v>144</v>
+        <v>183</v>
       </c>
       <c r="C71" s="107" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D71" s="108"/>
       <c r="E71" s="108"/>
       <c r="F71" s="108"/>
       <c r="G71" s="111"/>
-      <c r="H71" s="109">
-        <v>11</v>
+      <c r="H71" s="109" t="s">
+        <v>189</v>
       </c>
       <c r="I71" s="112"/>
       <c r="J71" s="112"/>
       <c r="K71" s="112" t="s">
-        <v>183</v>
-      </c>
-      <c r="L71" s="111"/>
-    </row>
-    <row r="72" spans="1:12" s="133" customFormat="1" ht="16.5">
-      <c r="A72" s="130">
-        <v>66</v>
-      </c>
-      <c r="B72" s="131" t="s">
-        <v>142</v>
-      </c>
-      <c r="C72" s="131" t="s">
-        <v>150</v>
-      </c>
-      <c r="D72" s="120"/>
-      <c r="E72" s="120"/>
-      <c r="F72" s="120"/>
-      <c r="G72" s="120"/>
-      <c r="H72" s="132" t="s">
-        <v>188</v>
-      </c>
-      <c r="I72" s="132"/>
-      <c r="J72" s="132"/>
-      <c r="K72" s="132"/>
-      <c r="L72" s="120"/>
-    </row>
-    <row r="73" spans="1:12" s="133" customFormat="1" ht="16.5">
-      <c r="A73" s="130">
-        <v>67</v>
-      </c>
-      <c r="B73" s="131" t="s">
-        <v>153</v>
-      </c>
-      <c r="C73" s="131" t="s">
-        <v>154</v>
-      </c>
-      <c r="D73" s="120"/>
-      <c r="E73" s="120"/>
-      <c r="F73" s="120"/>
-      <c r="G73" s="120"/>
-      <c r="H73" s="132" t="s">
-        <v>186</v>
-      </c>
-      <c r="I73" s="132"/>
-      <c r="J73" s="132"/>
-      <c r="K73" s="132"/>
-      <c r="L73" s="119">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" s="110" customFormat="1" ht="16.5">
-      <c r="A74" s="106">
+        <v>177</v>
+      </c>
+      <c r="L71" s="112"/>
+    </row>
+    <row r="72" spans="1:12" s="110" customFormat="1" ht="16.5">
+      <c r="A72" s="106">
+        <v>72</v>
+      </c>
+      <c r="B72" s="107" t="s">
+        <v>184</v>
+      </c>
+      <c r="C72" s="107" t="s">
+        <v>144</v>
+      </c>
+      <c r="D72" s="108"/>
+      <c r="E72" s="108"/>
+      <c r="F72" s="108"/>
+      <c r="G72" s="111"/>
+      <c r="H72" s="109" t="s">
+        <v>190</v>
+      </c>
+      <c r="I72" s="112"/>
+      <c r="J72" s="112"/>
+      <c r="K72" s="112" t="s">
+        <v>177</v>
+      </c>
+      <c r="L72" s="112"/>
+    </row>
+    <row r="73" spans="1:12" s="110" customFormat="1" ht="16.5">
+      <c r="A73" s="106">
+        <v>65</v>
+      </c>
+      <c r="B73" s="107" t="s">
+        <v>139</v>
+      </c>
+      <c r="C73" s="107" t="s">
+        <v>140</v>
+      </c>
+      <c r="D73" s="108"/>
+      <c r="E73" s="108"/>
+      <c r="F73" s="108"/>
+      <c r="G73" s="111"/>
+      <c r="H73" s="109" t="s">
+        <v>190</v>
+      </c>
+      <c r="I73" s="112"/>
+      <c r="J73" s="112"/>
+      <c r="K73" s="112"/>
+      <c r="L73" s="112" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" ht="16.5">
+      <c r="A74" s="83">
         <v>68</v>
       </c>
-      <c r="B74" s="107" t="s">
-        <v>167</v>
-      </c>
-      <c r="C74" s="107" t="s">
-        <v>168</v>
-      </c>
-      <c r="D74" s="108"/>
-      <c r="E74" s="108"/>
-      <c r="F74" s="108"/>
-      <c r="G74" s="111"/>
-      <c r="H74" s="109" t="s">
+      <c r="B74" s="82" t="s">
+        <v>161</v>
+      </c>
+      <c r="C74" s="82" t="s">
+        <v>162</v>
+      </c>
+      <c r="H74" s="86"/>
+      <c r="I74" s="136"/>
+      <c r="J74" s="123"/>
+      <c r="K74" s="123"/>
+      <c r="L74" s="123"/>
+    </row>
+    <row r="75" spans="1:12" ht="16.5">
+      <c r="A75" s="83">
+        <v>73</v>
+      </c>
+      <c r="B75" s="82" t="s">
         <v>185</v>
       </c>
-      <c r="I74" s="129"/>
-      <c r="J74" s="129"/>
-      <c r="K74" s="112" t="s">
-        <v>183</v>
-      </c>
-      <c r="L74" s="111"/>
+      <c r="H75" s="86"/>
+      <c r="I75" s="136"/>
+      <c r="J75" s="123"/>
+      <c r="K75" s="123"/>
+      <c r="L75" s="123"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3545,7 +3587,7 @@
     </row>
     <row r="33" spans="1:4" ht="16.5">
       <c r="A33" s="40" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B33" s="4">
         <v>0</v>
@@ -3559,7 +3601,7 @@
     </row>
     <row r="34" spans="1:4" ht="17.25" thickBot="1">
       <c r="A34" s="38" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B34" s="5">
         <v>1</v>
@@ -3629,7 +3671,7 @@
     </row>
     <row r="39" spans="1:4" ht="16.5">
       <c r="A39" s="40" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B39" s="4">
         <v>0</v>
@@ -3643,7 +3685,7 @@
     </row>
     <row r="40" spans="1:4" ht="17.25" thickBot="1">
       <c r="A40" s="38" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B40" s="5">
         <v>1</v>
@@ -3685,7 +3727,7 @@
     </row>
     <row r="43" spans="1:4" ht="16.5">
       <c r="A43" s="40" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B43" s="4">
         <v>0</v>
@@ -3699,7 +3741,7 @@
     </row>
     <row r="44" spans="1:4" ht="17.25" thickBot="1">
       <c r="A44" s="38" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B44" s="5">
         <v>1</v>
@@ -3713,7 +3755,7 @@
     </row>
     <row r="45" spans="1:4" ht="16.5">
       <c r="A45" s="40" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B45" s="4">
         <v>0</v>
@@ -3727,7 +3769,7 @@
     </row>
     <row r="46" spans="1:4" ht="17.25" thickBot="1">
       <c r="A46" s="38" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B46" s="5">
         <v>1</v>
@@ -3741,7 +3783,7 @@
     </row>
     <row r="47" spans="1:4" ht="16.5">
       <c r="A47" s="40" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B47" s="4">
         <v>0</v>
@@ -3755,7 +3797,7 @@
     </row>
     <row r="48" spans="1:4" ht="17.25" thickBot="1">
       <c r="A48" s="38" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B48" s="5">
         <v>1</v>
@@ -3769,7 +3811,7 @@
     </row>
     <row r="49" spans="1:4" ht="16.5">
       <c r="A49" s="40" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B49" s="4">
         <v>0</v>
@@ -3783,7 +3825,7 @@
     </row>
     <row r="50" spans="1:4" ht="17.25" thickBot="1">
       <c r="A50" s="38" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B50" s="5">
         <v>1</v>
@@ -3797,7 +3839,7 @@
     </row>
     <row r="51" spans="1:4" ht="16.5">
       <c r="A51" s="40" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B51" s="4">
         <v>0</v>
@@ -3811,7 +3853,7 @@
     </row>
     <row r="52" spans="1:4" ht="17.25" thickBot="1">
       <c r="A52" s="42" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B52" s="43">
         <v>1</v>
@@ -4027,10 +4069,10 @@
         <v>0</v>
       </c>
       <c r="C67" s="71" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D67" s="72" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15.75">

</xml_diff>

<commit_message>
Ara si que si (Esperem)
</commit_message>
<xml_diff>
--- a/conductor_DataHarmonization.xlsx
+++ b/conductor_DataHarmonization.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="19200" windowHeight="7395" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="19200" windowHeight="7395"/>
   </bookViews>
   <sheets>
     <sheet name="taulavariables" sheetId="8" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="226">
   <si>
     <t>id</t>
   </si>
@@ -398,9 +398,6 @@
     <t>Edad fecha índice [cataegorizada]</t>
   </si>
   <si>
-    <t>Edad fecha índice [categorizada]</t>
-  </si>
-  <si>
     <t>IMC [categorizado]</t>
   </si>
   <si>
@@ -690,6 +687,12 @@
   </si>
   <si>
     <t>Sujetos de grupos n&gt;5</t>
+  </si>
+  <si>
+    <t>Edad</t>
+  </si>
+  <si>
+    <t>Edad [categorizada]</t>
   </si>
 </sst>
 </file>
@@ -1296,7 +1299,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1306,11 +1309,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M76"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C71" sqref="C71"/>
+      <selection pane="bottomRight" activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -1341,7 +1344,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>3</v>
@@ -1353,22 +1356,22 @@
         <v>103</v>
       </c>
       <c r="H1" s="37" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I1" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="J1" s="42" t="s">
         <v>130</v>
       </c>
-      <c r="J1" s="42" t="s">
+      <c r="K1" s="42" t="s">
         <v>131</v>
       </c>
-      <c r="K1" s="42" t="s">
-        <v>132</v>
-      </c>
       <c r="L1" s="42" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M1" s="42" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="16.5">
@@ -1469,10 +1472,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="H8" s="37">
         <v>1</v>
@@ -1481,10 +1484,10 @@
     <row r="9" spans="1:13" s="36" customFormat="1" ht="16.5">
       <c r="A9" s="32"/>
       <c r="B9" s="33" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D9" s="33"/>
       <c r="E9" s="34"/>
@@ -1502,28 +1505,28 @@
     <row r="10" spans="1:13" ht="16.5">
       <c r="A10" s="2"/>
       <c r="B10" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="16.5">
       <c r="A11" s="2"/>
       <c r="B11" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:13" s="36" customFormat="1" ht="16.5">
       <c r="A12" s="32"/>
       <c r="B12" s="33" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D12" s="33"/>
       <c r="E12" s="34"/>
@@ -1539,10 +1542,10 @@
     <row r="13" spans="1:13" ht="16.5">
       <c r="A13" s="2"/>
       <c r="B13" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="14" spans="1:13" s="16" customFormat="1" ht="16.5">
@@ -1714,7 +1717,7 @@
         <v>121</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D21" s="13"/>
       <c r="E21" s="14"/>
@@ -1838,7 +1841,7 @@
         <v>28</v>
       </c>
       <c r="C30" s="21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D30" s="21" t="s">
         <v>76</v>
@@ -1860,10 +1863,10 @@
         <v>24</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D31" s="21" t="s">
         <v>77</v>
@@ -1888,7 +1891,7 @@
         <v>29</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D32" s="20" t="s">
         <v>78</v>
@@ -1913,7 +1916,7 @@
         <v>30</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D33" s="21" t="s">
         <v>79</v>
@@ -1935,10 +1938,10 @@
         <v>27</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D34" s="21" t="s">
         <v>80</v>
@@ -1963,7 +1966,7 @@
         <v>31</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D35" s="20" t="s">
         <v>81</v>
@@ -1985,10 +1988,10 @@
         <v>29</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D36" s="20" t="s">
         <v>82</v>
@@ -2010,10 +2013,10 @@
         <v>30</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D37" s="20" t="s">
         <v>83</v>
@@ -2035,13 +2038,13 @@
         <v>31</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C38" s="21" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D38" s="21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E38" s="22"/>
       <c r="F38" s="22">
@@ -2060,10 +2063,10 @@
         <v>32</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C39" s="21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D39" s="21" t="s">
         <v>84</v>
@@ -2085,13 +2088,13 @@
         <v>33</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D40" s="20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E40" s="22"/>
       <c r="F40" s="22">
@@ -2113,7 +2116,7 @@
         <v>32</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D41" s="21" t="s">
         <v>67</v>
@@ -2138,7 +2141,7 @@
         <v>33</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D42" s="21" t="s">
         <v>68</v>
@@ -2163,7 +2166,7 @@
         <v>34</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D43" s="20" t="s">
         <v>69</v>
@@ -2188,7 +2191,7 @@
         <v>35</v>
       </c>
       <c r="C44" s="21" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D44" s="21" t="s">
         <v>70</v>
@@ -2213,7 +2216,7 @@
         <v>36</v>
       </c>
       <c r="C45" s="21" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D45" s="21" t="s">
         <v>71</v>
@@ -2238,7 +2241,7 @@
         <v>37</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D46" s="20" t="s">
         <v>72</v>
@@ -2263,7 +2266,7 @@
         <v>38</v>
       </c>
       <c r="C47" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D47" s="20" t="s">
         <v>73</v>
@@ -2288,7 +2291,7 @@
         <v>39</v>
       </c>
       <c r="C48" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D48" s="20" t="s">
         <v>74</v>
@@ -2313,7 +2316,7 @@
         <v>40</v>
       </c>
       <c r="C49" s="21" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D49" s="21" t="s">
         <v>85</v>
@@ -2338,7 +2341,7 @@
         <v>41</v>
       </c>
       <c r="C50" s="21" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D50" s="21" t="s">
         <v>75</v>
@@ -2363,7 +2366,7 @@
         <v>42</v>
       </c>
       <c r="C51" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D51" s="20" t="s">
         <v>86</v>
@@ -2388,7 +2391,7 @@
         <v>43</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>87</v>
+        <v>224</v>
       </c>
       <c r="F52" s="6">
         <v>3</v>
@@ -2472,10 +2475,7 @@
         <v>106</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="F58" s="6">
-        <v>42</v>
+        <v>215</v>
       </c>
     </row>
     <row r="59" spans="1:13" ht="16.5">
@@ -2511,10 +2511,7 @@
         <v>109</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F61" s="6">
-        <v>43</v>
+        <v>145</v>
       </c>
     </row>
     <row r="62" spans="1:13" ht="16.5">
@@ -2525,7 +2522,7 @@
         <v>110</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>127</v>
+        <v>225</v>
       </c>
       <c r="F62" s="6">
         <v>44</v>
@@ -2536,10 +2533,10 @@
         <v>56</v>
       </c>
       <c r="B63" s="55" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C63" s="55" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D63" s="55"/>
       <c r="E63" s="56"/>
@@ -2550,10 +2547,10 @@
         <v>1</v>
       </c>
       <c r="J63" s="59" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K63" s="59" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L63" s="59"/>
       <c r="M63" s="59"/>
@@ -2563,10 +2560,10 @@
         <v>57</v>
       </c>
       <c r="B64" s="55" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C64" s="55" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D64" s="55"/>
       <c r="E64" s="56"/>
@@ -2590,10 +2587,10 @@
         <v>58</v>
       </c>
       <c r="B65" s="55" t="s">
+        <v>132</v>
+      </c>
+      <c r="C65" s="55" t="s">
         <v>133</v>
-      </c>
-      <c r="C65" s="55" t="s">
-        <v>134</v>
       </c>
       <c r="D65" s="55"/>
       <c r="E65" s="56"/>
@@ -2601,7 +2598,7 @@
       <c r="G65" s="56"/>
       <c r="H65" s="57"/>
       <c r="I65" s="58" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J65" s="61"/>
       <c r="K65" s="59">
@@ -2615,10 +2612,10 @@
         <v>63</v>
       </c>
       <c r="B66" s="26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C66" s="26" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D66" s="26"/>
       <c r="E66" s="27"/>
@@ -2626,12 +2623,12 @@
       <c r="G66" s="27"/>
       <c r="H66" s="30"/>
       <c r="I66" s="28" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J66" s="31"/>
       <c r="K66" s="31"/>
       <c r="L66" s="31" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M66" s="31"/>
     </row>
@@ -2640,25 +2637,25 @@
         <v>66</v>
       </c>
       <c r="B67" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C67" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D67" s="26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E67" s="27"/>
       <c r="F67" s="27"/>
       <c r="G67" s="27"/>
       <c r="H67" s="30"/>
       <c r="I67" s="28" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J67" s="31"/>
       <c r="K67" s="31"/>
       <c r="L67" s="31" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M67" s="31"/>
     </row>
@@ -2667,25 +2664,25 @@
         <v>67</v>
       </c>
       <c r="B68" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="C68" s="26" t="s">
+        <v>221</v>
+      </c>
+      <c r="D68" s="26" t="s">
         <v>144</v>
-      </c>
-      <c r="C68" s="26" t="s">
-        <v>222</v>
-      </c>
-      <c r="D68" s="26" t="s">
-        <v>145</v>
       </c>
       <c r="E68" s="27"/>
       <c r="F68" s="27"/>
       <c r="G68" s="27"/>
       <c r="H68" s="30"/>
       <c r="I68" s="28" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J68" s="31"/>
       <c r="K68" s="31"/>
       <c r="L68" s="31" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M68" s="31"/>
     </row>
@@ -2694,13 +2691,13 @@
         <v>69</v>
       </c>
       <c r="B69" s="26" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C69" s="26" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D69" s="26" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E69" s="27"/>
       <c r="F69" s="27">
@@ -2709,12 +2706,12 @@
       <c r="G69" s="27"/>
       <c r="H69" s="30"/>
       <c r="I69" s="28" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J69" s="31"/>
       <c r="K69" s="31"/>
       <c r="L69" s="31" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M69" s="31"/>
     </row>
@@ -2723,13 +2720,13 @@
         <v>70</v>
       </c>
       <c r="B70" s="26" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C70" s="26" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D70" s="26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E70" s="27"/>
       <c r="F70" s="27">
@@ -2738,12 +2735,12 @@
       <c r="G70" s="27"/>
       <c r="H70" s="30"/>
       <c r="I70" s="28" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J70" s="31"/>
       <c r="K70" s="31"/>
       <c r="L70" s="31" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M70" s="31"/>
     </row>
@@ -2752,13 +2749,13 @@
         <v>71</v>
       </c>
       <c r="B71" s="26" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C71" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D71" s="26" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E71" s="27"/>
       <c r="F71" s="27">
@@ -2767,12 +2764,12 @@
       <c r="G71" s="27"/>
       <c r="H71" s="30"/>
       <c r="I71" s="28" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J71" s="31"/>
       <c r="K71" s="31"/>
       <c r="L71" s="31" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M71" s="31"/>
     </row>
@@ -2781,13 +2778,13 @@
         <v>72</v>
       </c>
       <c r="B72" s="26" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C72" s="26" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D72" s="26" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E72" s="27"/>
       <c r="F72" s="27">
@@ -2796,12 +2793,12 @@
       <c r="G72" s="27"/>
       <c r="H72" s="30"/>
       <c r="I72" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J72" s="31"/>
       <c r="K72" s="31"/>
       <c r="L72" s="31" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M72" s="31"/>
     </row>
@@ -2810,26 +2807,26 @@
         <v>65</v>
       </c>
       <c r="B73" s="48" t="s">
+        <v>136</v>
+      </c>
+      <c r="C73" s="48" t="s">
+        <v>223</v>
+      </c>
+      <c r="D73" s="48" t="s">
         <v>137</v>
-      </c>
-      <c r="C73" s="48" t="s">
-        <v>224</v>
-      </c>
-      <c r="D73" s="48" t="s">
-        <v>138</v>
       </c>
       <c r="E73" s="49"/>
       <c r="F73" s="49"/>
       <c r="G73" s="49"/>
       <c r="H73" s="50"/>
       <c r="I73" s="51" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J73" s="52"/>
       <c r="K73" s="52"/>
       <c r="L73" s="52"/>
       <c r="M73" s="52" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="74" spans="1:13" ht="16.5">
@@ -2837,10 +2834,10 @@
         <v>68</v>
       </c>
       <c r="B74" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C74" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>158</v>
       </c>
       <c r="I74" s="5"/>
       <c r="J74" s="62"/>
@@ -2853,7 +2850,7 @@
         <v>73</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I75" s="5"/>
       <c r="J75" s="62"/>
@@ -2866,10 +2863,10 @@
         <v>74</v>
       </c>
       <c r="B76" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C76" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>192</v>
       </c>
       <c r="F76" s="6">
         <v>49</v>
@@ -2885,11 +2882,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomRight" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2934,7 +2931,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="63" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D2" s="63" t="s">
         <v>45</v>
@@ -2948,7 +2945,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="63" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D3" s="63" t="s">
         <v>46</v>
@@ -3018,10 +3015,10 @@
         <v>53</v>
       </c>
       <c r="C8" s="63" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D8" s="63" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75">
@@ -3362,7 +3359,7 @@
     </row>
     <row r="33" spans="1:4" ht="15.75">
       <c r="A33" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B33" s="63">
         <v>0</v>
@@ -3376,7 +3373,7 @@
     </row>
     <row r="34" spans="1:4" ht="15.75">
       <c r="A34" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B34" s="63">
         <v>1</v>
@@ -3446,7 +3443,7 @@
     </row>
     <row r="39" spans="1:4" ht="15.75">
       <c r="A39" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B39" s="63">
         <v>0</v>
@@ -3460,7 +3457,7 @@
     </row>
     <row r="40" spans="1:4" ht="15.75">
       <c r="A40" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B40" s="63">
         <v>1</v>
@@ -3502,7 +3499,7 @@
     </row>
     <row r="43" spans="1:4" ht="15.75">
       <c r="A43" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B43" s="63">
         <v>0</v>
@@ -3516,7 +3513,7 @@
     </row>
     <row r="44" spans="1:4" ht="15.75">
       <c r="A44" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B44" s="63">
         <v>1</v>
@@ -3530,7 +3527,7 @@
     </row>
     <row r="45" spans="1:4" ht="15.75">
       <c r="A45" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B45" s="63">
         <v>0</v>
@@ -3544,7 +3541,7 @@
     </row>
     <row r="46" spans="1:4" ht="15.75">
       <c r="A46" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B46" s="63">
         <v>1</v>
@@ -3558,7 +3555,7 @@
     </row>
     <row r="47" spans="1:4" ht="15.75">
       <c r="A47" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B47" s="63">
         <v>0</v>
@@ -3572,7 +3569,7 @@
     </row>
     <row r="48" spans="1:4" ht="15.75">
       <c r="A48" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B48" s="63">
         <v>1</v>
@@ -3586,7 +3583,7 @@
     </row>
     <row r="49" spans="1:4" ht="15.75">
       <c r="A49" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B49" s="63">
         <v>0</v>
@@ -3600,7 +3597,7 @@
     </row>
     <row r="50" spans="1:4" ht="15.75">
       <c r="A50" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B50" s="63">
         <v>1</v>
@@ -3614,7 +3611,7 @@
     </row>
     <row r="51" spans="1:4" ht="15.75">
       <c r="A51" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B51" s="63">
         <v>0</v>
@@ -3628,7 +3625,7 @@
     </row>
     <row r="52" spans="1:4" ht="15.75">
       <c r="A52" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B52" s="63">
         <v>1</v>
@@ -3844,10 +3841,10 @@
         <v>0</v>
       </c>
       <c r="C67" s="63" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D67" s="63" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -3922,7 +3919,7 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="64" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B73" s="63">
         <v>0</v>
@@ -3936,7 +3933,7 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="64" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B74" s="63">
         <v>1</v>
@@ -3950,7 +3947,7 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="64" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B75" s="63">
         <v>0</v>
@@ -3964,7 +3961,7 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="64" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B76" s="63">
         <v>1</v>
@@ -3978,7 +3975,7 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="64" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B77" s="63">
         <v>0</v>
@@ -3992,7 +3989,7 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="64" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B78" s="63">
         <v>1</v>
@@ -4006,7 +4003,7 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="64" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B79" s="63">
         <v>0</v>
@@ -4020,7 +4017,7 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="64" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B80" s="63">
         <v>1</v>

</xml_diff>